<commit_message>
Send an email report when a path is closed
</commit_message>
<xml_diff>
--- a/BreadingBread.Infraestructure/Reportes/PlantillaBasico.xlsx
+++ b/BreadingBread.Infraestructure/Reportes/PlantillaBasico.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Fecha : </t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>Nombre de repartidor</t>
+  </si>
+  <si>
+    <t>Ruta:</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -68,11 +74,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,33 +361,38 @@
   <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C3" s="1">
         <v>43692</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="3"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>

</xml_diff>